<commit_message>
hopefully pay attention to files removed
</commit_message>
<xml_diff>
--- a/NetworkData/NetworkTests.xlsx
+++ b/NetworkData/NetworkTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13240" tabRatio="500"/>
+    <workbookView xWindow="28840" yWindow="-3600" windowWidth="20140" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5080" ySplit="560" topLeftCell="D2" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
added a script to query enrichr
</commit_message>
<xml_diff>
--- a/NetworkData/NetworkTests.xlsx
+++ b/NetworkData/NetworkTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28840" yWindow="-3600" windowWidth="20140" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="-20" windowWidth="36280" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,8 +224,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -337,7 +345,7 @@
     <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +371,10 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -388,6 +400,10 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -720,10 +736,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5080" ySplit="560" topLeftCell="D2" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>